<commit_message>
Updated paths on dbpedia-en demo
</commit_message>
<xml_diff>
--- a/demos/demo-dbpedia-en/sparnatural-config.xlsx
+++ b/demos/demo-dbpedia-en/sparnatural-config.xlsx
@@ -15,6 +15,9 @@
     <sheet name="sparnatural-config-core" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
+  </extLst>
 </workbook>
 </file>
 
@@ -668,7 +671,7 @@
     <t>this:Artwork_displayedAt</t>
   </si>
   <si>
-    <t xml:space="preserve">[sh:alternativePath (dbpedia:museum [sh:inversePath dbpedia:displays])]</t>
+    <t>dbpedia:museum|^dbpedia:displays</t>
   </si>
   <si>
     <t xml:space="preserve">displayed at</t>
@@ -704,7 +707,7 @@
     <t>this:Museum_country</t>
   </si>
   <si>
-    <t>dbpedia:country</t>
+    <t>dbpedia:location/dbpedia:country</t>
   </si>
   <si>
     <t>country</t>
@@ -743,7 +746,7 @@
     <t>this:Museum_displays</t>
   </si>
   <si>
-    <t xml:space="preserve">[sh:alternativePath (dbpedia:displays [sh:inversePath dbpedia:museum])]</t>
+    <t>dbpedia:displays|^dbpedia:museum</t>
   </si>
   <si>
     <t>displays</t>
@@ -781,7 +784,7 @@
     <t>this:Country_countryOf</t>
   </si>
   <si>
-    <t xml:space="preserve">[ sh:inversePath dbpedia:country ]</t>
+    <t>^dbpedia:country/^dbpedia:location</t>
   </si>
   <si>
     <t xml:space="preserve">country of</t>
@@ -802,7 +805,7 @@
     <t>this:Country_deathPlace</t>
   </si>
   <si>
-    <t xml:space="preserve">[ sh:inversePath  dbpedia:deathPlace ]</t>
+    <t>^dbpedia:deathPlace</t>
   </si>
   <si>
     <t xml:space="preserve">death place of</t>
@@ -820,7 +823,7 @@
     <t>this:Country_birthPlace</t>
   </si>
   <si>
-    <t xml:space="preserve">[ sh:inversePath  dbpedia:birthPlace ]</t>
+    <t>^dbpedia:birthPlace</t>
   </si>
   <si>
     <t xml:space="preserve">birth place of</t>
@@ -838,7 +841,7 @@
     <t>this:Person_bornIn</t>
   </si>
   <si>
-    <t xml:space="preserve">(dbpedia:birthPlace dbpedia:country)</t>
+    <t>dbpedia:birthPlace/dbpedia:country</t>
   </si>
   <si>
     <t xml:space="preserve">born in</t>
@@ -853,7 +856,7 @@
     <t>this:Person_diedIn</t>
   </si>
   <si>
-    <t xml:space="preserve">(dbpedia:deathPlace dbpedia:country)</t>
+    <t>dbpedia:deathPlace/dbpedia:country</t>
   </si>
   <si>
     <t xml:space="preserve">died in</t>
@@ -910,7 +913,7 @@
     <t>this:Person_created</t>
   </si>
   <si>
-    <t xml:space="preserve">[ sh:inversePath dbpedia:author ]</t>
+    <t>^dbpedia:author</t>
   </si>
   <si>
     <t>created</t>
@@ -958,7 +961,7 @@
     <t>this:Movement_movementIncludes</t>
   </si>
   <si>
-    <t xml:space="preserve">[ sh:inversePath dbpedia:movement ]</t>
+    <t>^dbpedia:movement</t>
   </si>
   <si>
     <t>participant</t>

</xml_diff>